<commit_message>
add ETL to Line
</commit_message>
<xml_diff>
--- a/ETL/Data/data.xlsx
+++ b/ETL/Data/data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/galigaribaldi/Documents/PPropios/API Tren/Apimetro/ETL/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55789506-1252-5640-A80A-03AD85954682}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B6D7F9D-9CDC-874E-9E9A-70E0D29267D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="68800" yWindow="500" windowWidth="38400" windowHeight="19400" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1980" uniqueCount="637">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2029" uniqueCount="676">
   <si>
     <t>SISTEMA</t>
   </si>
@@ -1935,16 +1935,139 @@
   </si>
   <si>
     <t>PINK</t>
+  </si>
+  <si>
+    <t>LINEA_ID</t>
+  </si>
+  <si>
+    <t>ANIO_INAUGURACION</t>
+  </si>
+  <si>
+    <t>AZUL</t>
+  </si>
+  <si>
+    <t>BLUE</t>
+  </si>
+  <si>
+    <t>VERDE_OLIVO</t>
+  </si>
+  <si>
+    <t>OLIVE_GREEN</t>
+  </si>
+  <si>
+    <t>TAM_KM</t>
+  </si>
+  <si>
+    <t>CIAN</t>
+  </si>
+  <si>
+    <t>CYAN</t>
+  </si>
+  <si>
+    <t>AFLUENCIA</t>
+  </si>
+  <si>
+    <t>BAJA</t>
+  </si>
+  <si>
+    <t>AMARILLO</t>
+  </si>
+  <si>
+    <t>YELLOW</t>
+  </si>
+  <si>
+    <t>ROJO</t>
+  </si>
+  <si>
+    <t>RED</t>
+  </si>
+  <si>
+    <t>NARANJA</t>
+  </si>
+  <si>
+    <t>ORANGE</t>
+  </si>
+  <si>
+    <t>GREEN</t>
+  </si>
+  <si>
+    <t>VERDE</t>
+  </si>
+  <si>
+    <t>CAFÉ</t>
+  </si>
+  <si>
+    <t>BROWN</t>
+  </si>
+  <si>
+    <t>DORADO</t>
+  </si>
+  <si>
+    <t>GOLDEN</t>
+  </si>
+  <si>
+    <t>LINEA 1</t>
+  </si>
+  <si>
+    <t>LINEA 2</t>
+  </si>
+  <si>
+    <t>LINEA 3</t>
+  </si>
+  <si>
+    <t>LINEA 4</t>
+  </si>
+  <si>
+    <t>LINEA 5</t>
+  </si>
+  <si>
+    <t>LINEA 6</t>
+  </si>
+  <si>
+    <t>LINEA 7</t>
+  </si>
+  <si>
+    <t>LINEA 8</t>
+  </si>
+  <si>
+    <t>LINEA 9</t>
+  </si>
+  <si>
+    <t>LINEA 12</t>
+  </si>
+  <si>
+    <t>LINEA A</t>
+  </si>
+  <si>
+    <t>MORADA</t>
+  </si>
+  <si>
+    <t>PURPLE</t>
+  </si>
+  <si>
+    <t>LINEA B</t>
+  </si>
+  <si>
+    <t>VERDE_GRIS</t>
+  </si>
+  <si>
+    <t>GREEN_GREY</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -9115,6 +9238,12 @@
   </sheetData>
   <autoFilter ref="A1:K196" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <mergeCells count="14">
+    <mergeCell ref="M71:M72"/>
+    <mergeCell ref="M75:M76"/>
+    <mergeCell ref="M56:M57"/>
+    <mergeCell ref="M49:M50"/>
+    <mergeCell ref="M63:M64"/>
+    <mergeCell ref="M65:M66"/>
     <mergeCell ref="N65:N66"/>
     <mergeCell ref="O65:O66"/>
     <mergeCell ref="M8:M9"/>
@@ -9123,12 +9252,6 @@
     <mergeCell ref="M18:M19"/>
     <mergeCell ref="M20:M21"/>
     <mergeCell ref="N20:N21"/>
-    <mergeCell ref="M71:M72"/>
-    <mergeCell ref="M75:M76"/>
-    <mergeCell ref="M56:M57"/>
-    <mergeCell ref="M49:M50"/>
-    <mergeCell ref="M63:M64"/>
-    <mergeCell ref="M65:M66"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -9137,49 +9260,321 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D61F9FF-1099-874D-861D-4522CE1B5818}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>2</v>
+        <v>637</v>
       </c>
       <c r="C1" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D1" t="s">
+        <v>638</v>
+      </c>
+      <c r="E1" t="s">
         <v>633</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>634</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G1" t="s">
+        <v>643</v>
+      </c>
+      <c r="H1" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
-      <c r="C2">
+      <c r="C2" t="s">
+        <v>660</v>
+      </c>
+      <c r="D2">
         <v>1969</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>635</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>636</v>
       </c>
+      <c r="G2">
+        <v>18.8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>661</v>
+      </c>
+      <c r="D3">
+        <v>1970</v>
+      </c>
+      <c r="E3" t="s">
+        <v>639</v>
+      </c>
+      <c r="F3" t="s">
+        <v>640</v>
+      </c>
+      <c r="G3">
+        <v>23.43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>662</v>
+      </c>
+      <c r="D4">
+        <v>1970</v>
+      </c>
+      <c r="E4" t="s">
+        <v>641</v>
+      </c>
+      <c r="F4" t="s">
+        <v>642</v>
+      </c>
+      <c r="G4">
+        <v>23.61</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>663</v>
+      </c>
+      <c r="D5">
+        <v>1981</v>
+      </c>
+      <c r="E5" t="s">
+        <v>644</v>
+      </c>
+      <c r="F5" t="s">
+        <v>645</v>
+      </c>
+      <c r="G5">
+        <v>10.75</v>
+      </c>
+      <c r="H5" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>664</v>
+      </c>
+      <c r="D6">
+        <v>1981</v>
+      </c>
+      <c r="E6" t="s">
+        <v>648</v>
+      </c>
+      <c r="F6" t="s">
+        <v>649</v>
+      </c>
+      <c r="G6">
+        <v>16.670000000000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>665</v>
+      </c>
+      <c r="D7">
+        <v>1983</v>
+      </c>
+      <c r="E7" t="s">
+        <v>650</v>
+      </c>
+      <c r="F7" t="s">
+        <v>651</v>
+      </c>
+      <c r="G7">
+        <v>13.95</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
+        <v>666</v>
+      </c>
+      <c r="D8">
+        <v>1984</v>
+      </c>
+      <c r="E8" t="s">
+        <v>652</v>
+      </c>
+      <c r="F8" t="s">
+        <v>653</v>
+      </c>
+      <c r="G8">
+        <v>18.78</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9" t="s">
+        <v>667</v>
+      </c>
+      <c r="D9">
+        <v>1994</v>
+      </c>
+      <c r="E9" t="s">
+        <v>655</v>
+      </c>
+      <c r="F9" t="s">
+        <v>654</v>
+      </c>
+      <c r="G9">
+        <v>20.079999999999998</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10">
+        <v>9</v>
+      </c>
+      <c r="C10" t="s">
+        <v>668</v>
+      </c>
+      <c r="D10">
+        <v>1987</v>
+      </c>
+      <c r="E10" t="s">
+        <v>656</v>
+      </c>
+      <c r="F10" t="s">
+        <v>657</v>
+      </c>
+      <c r="G10">
+        <v>15.37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11" t="s">
+        <v>670</v>
+      </c>
+      <c r="D11">
+        <v>1991</v>
+      </c>
+      <c r="E11" t="s">
+        <v>671</v>
+      </c>
+      <c r="F11" t="s">
+        <v>672</v>
+      </c>
+      <c r="G11">
+        <v>17.190000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12">
+        <v>11</v>
+      </c>
+      <c r="C12" t="s">
+        <v>673</v>
+      </c>
+      <c r="D12">
+        <v>1999</v>
+      </c>
+      <c r="E12" t="s">
+        <v>674</v>
+      </c>
+      <c r="F12" t="s">
+        <v>675</v>
+      </c>
+      <c r="G12">
+        <v>23.72</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13">
+        <v>12</v>
+      </c>
+      <c r="C13" t="s">
+        <v>669</v>
+      </c>
+      <c r="D13">
+        <v>2012</v>
+      </c>
+      <c r="E13" t="s">
+        <v>658</v>
+      </c>
+      <c r="F13" t="s">
+        <v>659</v>
+      </c>
+      <c r="G13">
+        <v>24.5</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
modify Routes and ETL
</commit_message>
<xml_diff>
--- a/ETL/Data/data.xlsx
+++ b/ETL/Data/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/galigaribaldi/Documents/PPropios/API Tren/Apimetro/ETL/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA7FD1ED-BDE9-1A42-8F1D-F65AAC1C66FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4460F33-C24E-DB45-AA7C-051A55EDF558}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="68800" yWindow="500" windowWidth="38400" windowHeight="19400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2097,13 +2097,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2404,7 +2404,7 @@
   <dimension ref="A1:O196"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="H213" sqref="H213"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2720,7 +2720,7 @@
       <c r="L8" t="s">
         <v>619</v>
       </c>
-      <c r="M8" s="3" t="s">
+      <c r="M8" s="2" t="s">
         <v>626</v>
       </c>
     </row>
@@ -2761,7 +2761,7 @@
       <c r="L9" t="s">
         <v>619</v>
       </c>
-      <c r="M9" s="3"/>
+      <c r="M9" s="2"/>
     </row>
     <row r="10" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
@@ -2800,7 +2800,7 @@
       <c r="L10" t="s">
         <v>619</v>
       </c>
-      <c r="M10" s="3" t="s">
+      <c r="M10" s="2" t="s">
         <v>626</v>
       </c>
     </row>
@@ -2841,7 +2841,7 @@
       <c r="L11" t="s">
         <v>619</v>
       </c>
-      <c r="M11" s="3"/>
+      <c r="M11" s="2"/>
     </row>
     <row r="12" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
@@ -2880,7 +2880,7 @@
       <c r="L12" t="s">
         <v>619</v>
       </c>
-      <c r="M12" s="3" t="s">
+      <c r="M12" s="2" t="s">
         <v>626</v>
       </c>
     </row>
@@ -2921,7 +2921,7 @@
       <c r="L13" t="s">
         <v>619</v>
       </c>
-      <c r="M13" s="3"/>
+      <c r="M13" s="2"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
@@ -3112,7 +3112,7 @@
       <c r="L18" t="s">
         <v>619</v>
       </c>
-      <c r="M18" s="3" t="s">
+      <c r="M18" s="2" t="s">
         <v>626</v>
       </c>
     </row>
@@ -3153,7 +3153,7 @@
       <c r="L19" t="s">
         <v>619</v>
       </c>
-      <c r="M19" s="3"/>
+      <c r="M19" s="2"/>
     </row>
     <row r="20" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
@@ -3192,10 +3192,10 @@
       <c r="L20" t="s">
         <v>619</v>
       </c>
-      <c r="M20" s="3" t="s">
+      <c r="M20" s="2" t="s">
         <v>626</v>
       </c>
-      <c r="N20" s="3" t="s">
+      <c r="N20" s="2" t="s">
         <v>626</v>
       </c>
     </row>
@@ -3236,8 +3236,8 @@
       <c r="L21" t="s">
         <v>619</v>
       </c>
-      <c r="M21" s="3"/>
-      <c r="N21" s="3"/>
+      <c r="M21" s="2"/>
+      <c r="N21" s="2"/>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
@@ -4302,7 +4302,7 @@
       <c r="L49" t="s">
         <v>619</v>
       </c>
-      <c r="M49" s="3" t="s">
+      <c r="M49" s="2" t="s">
         <v>626</v>
       </c>
     </row>
@@ -4343,7 +4343,7 @@
       <c r="L50" t="s">
         <v>619</v>
       </c>
-      <c r="M50" s="3"/>
+      <c r="M50" s="2"/>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
@@ -4572,7 +4572,7 @@
       <c r="L56" t="s">
         <v>619</v>
       </c>
-      <c r="M56" s="3" t="s">
+      <c r="M56" s="2" t="s">
         <v>626</v>
       </c>
     </row>
@@ -4613,7 +4613,7 @@
       <c r="L57" t="s">
         <v>619</v>
       </c>
-      <c r="M57" s="3"/>
+      <c r="M57" s="2"/>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
@@ -4842,7 +4842,7 @@
       <c r="L63" t="s">
         <v>619</v>
       </c>
-      <c r="M63" s="3" t="s">
+      <c r="M63" s="2" t="s">
         <v>626</v>
       </c>
     </row>
@@ -4883,7 +4883,7 @@
       <c r="L64" t="s">
         <v>619</v>
       </c>
-      <c r="M64" s="3"/>
+      <c r="M64" s="2"/>
     </row>
     <row r="65" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
@@ -4922,13 +4922,13 @@
       <c r="L65" t="s">
         <v>619</v>
       </c>
-      <c r="M65" s="3" t="s">
+      <c r="M65" s="2" t="s">
         <v>626</v>
       </c>
-      <c r="N65" s="3" t="s">
+      <c r="N65" s="2" t="s">
         <v>626</v>
       </c>
-      <c r="O65" s="3" t="s">
+      <c r="O65" s="2" t="s">
         <v>626</v>
       </c>
     </row>
@@ -4969,9 +4969,9 @@
       <c r="L66" t="s">
         <v>619</v>
       </c>
-      <c r="M66" s="3"/>
-      <c r="N66" s="3"/>
-      <c r="O66" s="3"/>
+      <c r="M66" s="2"/>
+      <c r="N66" s="2"/>
+      <c r="O66" s="2"/>
     </row>
     <row r="67" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
@@ -5162,7 +5162,7 @@
       <c r="L71" t="s">
         <v>619</v>
       </c>
-      <c r="M71" s="3" t="s">
+      <c r="M71" s="2" t="s">
         <v>626</v>
       </c>
     </row>
@@ -5203,7 +5203,7 @@
       <c r="L72" t="s">
         <v>619</v>
       </c>
-      <c r="M72" s="3"/>
+      <c r="M72" s="2"/>
     </row>
     <row r="73" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
@@ -5318,7 +5318,7 @@
       <c r="L75" t="s">
         <v>619</v>
       </c>
-      <c r="M75" s="3" t="s">
+      <c r="M75" s="2" t="s">
         <v>626</v>
       </c>
     </row>
@@ -5359,7 +5359,7 @@
       <c r="L76" t="s">
         <v>619</v>
       </c>
-      <c r="M76" s="3"/>
+      <c r="M76" s="2"/>
     </row>
     <row r="77" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
@@ -5474,7 +5474,7 @@
       <c r="L79" t="s">
         <v>619</v>
       </c>
-      <c r="M79" s="4" t="s">
+      <c r="M79" s="3" t="s">
         <v>626</v>
       </c>
     </row>
@@ -5515,7 +5515,7 @@
       <c r="L80" t="s">
         <v>619</v>
       </c>
-      <c r="M80" s="4"/>
+      <c r="M80" s="3"/>
     </row>
     <row r="81" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
@@ -5554,7 +5554,7 @@
       <c r="L81" t="s">
         <v>619</v>
       </c>
-      <c r="M81" s="4"/>
+      <c r="M81" s="3"/>
     </row>
     <row r="82" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
@@ -5593,7 +5593,7 @@
       <c r="L82" t="s">
         <v>619</v>
       </c>
-      <c r="M82" s="4" t="s">
+      <c r="M82" s="3" t="s">
         <v>626</v>
       </c>
     </row>
@@ -5634,7 +5634,7 @@
       <c r="L83" t="s">
         <v>619</v>
       </c>
-      <c r="M83" s="4"/>
+      <c r="M83" s="3"/>
     </row>
     <row r="84" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
@@ -5673,7 +5673,7 @@
       <c r="L84" t="s">
         <v>619</v>
       </c>
-      <c r="M84" s="4"/>
+      <c r="M84" s="3"/>
     </row>
     <row r="85" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
@@ -5712,7 +5712,7 @@
       <c r="L85" t="s">
         <v>619</v>
       </c>
-      <c r="M85" s="4"/>
+      <c r="M85" s="3"/>
     </row>
     <row r="86" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
@@ -5751,7 +5751,7 @@
       <c r="L86" t="s">
         <v>619</v>
       </c>
-      <c r="M86" s="4"/>
+      <c r="M86" s="3"/>
     </row>
     <row r="87" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
@@ -5790,7 +5790,7 @@
       <c r="L87" t="s">
         <v>619</v>
       </c>
-      <c r="M87" s="3" t="s">
+      <c r="M87" s="2" t="s">
         <v>626</v>
       </c>
     </row>
@@ -5831,7 +5831,7 @@
       <c r="L88" t="s">
         <v>619</v>
       </c>
-      <c r="M88" s="3"/>
+      <c r="M88" s="2"/>
     </row>
     <row r="89" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
@@ -5908,7 +5908,7 @@
       <c r="L90" t="s">
         <v>619</v>
       </c>
-      <c r="M90" s="3" t="s">
+      <c r="M90" s="2" t="s">
         <v>626</v>
       </c>
     </row>
@@ -5949,7 +5949,7 @@
       <c r="L91" t="s">
         <v>619</v>
       </c>
-      <c r="M91" s="3"/>
+      <c r="M91" s="2"/>
     </row>
     <row r="92" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
@@ -5988,7 +5988,7 @@
       <c r="L92" t="s">
         <v>619</v>
       </c>
-      <c r="M92" s="3" t="s">
+      <c r="M92" s="2" t="s">
         <v>626</v>
       </c>
     </row>
@@ -6029,7 +6029,7 @@
       <c r="L93" t="s">
         <v>619</v>
       </c>
-      <c r="M93" s="3"/>
+      <c r="M93" s="2"/>
     </row>
     <row r="94" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
@@ -6068,7 +6068,7 @@
       <c r="L94" t="s">
         <v>619</v>
       </c>
-      <c r="M94" s="3" t="s">
+      <c r="M94" s="2" t="s">
         <v>626</v>
       </c>
     </row>
@@ -6109,7 +6109,7 @@
       <c r="L95" t="s">
         <v>619</v>
       </c>
-      <c r="M95" s="3"/>
+      <c r="M95" s="2"/>
     </row>
     <row r="96" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
@@ -6148,7 +6148,7 @@
       <c r="L96" t="s">
         <v>619</v>
       </c>
-      <c r="M96" s="3" t="s">
+      <c r="M96" s="2" t="s">
         <v>626</v>
       </c>
     </row>
@@ -6189,7 +6189,7 @@
       <c r="L97" t="s">
         <v>619</v>
       </c>
-      <c r="M97" s="3"/>
+      <c r="M97" s="2"/>
     </row>
     <row r="98" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
@@ -6228,7 +6228,7 @@
       <c r="L98" t="s">
         <v>619</v>
       </c>
-      <c r="M98" s="3" t="s">
+      <c r="M98" s="2" t="s">
         <v>626</v>
       </c>
     </row>
@@ -6269,7 +6269,7 @@
       <c r="L99" t="s">
         <v>619</v>
       </c>
-      <c r="M99" s="3"/>
+      <c r="M99" s="2"/>
     </row>
     <row r="100" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
@@ -6308,7 +6308,7 @@
       <c r="L100" t="s">
         <v>619</v>
       </c>
-      <c r="M100" s="3"/>
+      <c r="M100" s="2"/>
     </row>
     <row r="101" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
@@ -6347,7 +6347,7 @@
       <c r="L101" t="s">
         <v>619</v>
       </c>
-      <c r="M101" s="3" t="s">
+      <c r="M101" s="2" t="s">
         <v>626</v>
       </c>
     </row>
@@ -6388,8 +6388,8 @@
       <c r="L102" t="s">
         <v>619</v>
       </c>
-      <c r="M102" s="3"/>
-      <c r="N102" s="3" t="s">
+      <c r="M102" s="2"/>
+      <c r="N102" s="2" t="s">
         <v>626</v>
       </c>
     </row>
@@ -6430,7 +6430,7 @@
       <c r="L103" t="s">
         <v>619</v>
       </c>
-      <c r="N103" s="3"/>
+      <c r="N103" s="2"/>
     </row>
     <row r="104" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
@@ -6469,7 +6469,7 @@
       <c r="L104" t="s">
         <v>619</v>
       </c>
-      <c r="M104" s="3" t="s">
+      <c r="M104" s="2" t="s">
         <v>626</v>
       </c>
     </row>
@@ -6510,7 +6510,7 @@
       <c r="L105" t="s">
         <v>619</v>
       </c>
-      <c r="M105" s="3"/>
+      <c r="M105" s="2"/>
     </row>
     <row r="106" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
@@ -6549,7 +6549,7 @@
       <c r="L106" t="s">
         <v>619</v>
       </c>
-      <c r="M106" s="3" t="s">
+      <c r="M106" s="2" t="s">
         <v>626</v>
       </c>
     </row>
@@ -6590,7 +6590,7 @@
       <c r="L107" t="s">
         <v>619</v>
       </c>
-      <c r="M107" s="3"/>
+      <c r="M107" s="2"/>
     </row>
     <row r="108" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
@@ -6667,7 +6667,7 @@
       <c r="L109" t="s">
         <v>619</v>
       </c>
-      <c r="M109" s="3" t="s">
+      <c r="M109" s="2" t="s">
         <v>626</v>
       </c>
     </row>
@@ -6708,7 +6708,7 @@
       <c r="L110" t="s">
         <v>619</v>
       </c>
-      <c r="M110" s="3"/>
+      <c r="M110" s="2"/>
     </row>
     <row r="111" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
@@ -7089,7 +7089,7 @@
       <c r="L120" t="s">
         <v>619</v>
       </c>
-      <c r="M120" s="3" t="s">
+      <c r="M120" s="2" t="s">
         <v>626</v>
       </c>
     </row>
@@ -7130,7 +7130,7 @@
       <c r="L121" t="s">
         <v>619</v>
       </c>
-      <c r="M121" s="3"/>
+      <c r="M121" s="2"/>
     </row>
     <row r="122" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
@@ -7169,7 +7169,7 @@
       <c r="L122" t="s">
         <v>619</v>
       </c>
-      <c r="M122" s="3" t="s">
+      <c r="M122" s="2" t="s">
         <v>626</v>
       </c>
     </row>
@@ -7210,7 +7210,7 @@
       <c r="L123" t="s">
         <v>619</v>
       </c>
-      <c r="M123" s="3"/>
+      <c r="M123" s="2"/>
     </row>
     <row r="124" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
@@ -7249,7 +7249,7 @@
       <c r="L124" t="s">
         <v>619</v>
       </c>
-      <c r="M124" s="3" t="s">
+      <c r="M124" s="2" t="s">
         <v>626</v>
       </c>
     </row>
@@ -7290,7 +7290,7 @@
       <c r="L125" t="s">
         <v>619</v>
       </c>
-      <c r="M125" s="3"/>
+      <c r="M125" s="2"/>
     </row>
     <row r="126" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
@@ -7405,7 +7405,7 @@
       <c r="L128" t="s">
         <v>619</v>
       </c>
-      <c r="M128" s="3" t="s">
+      <c r="M128" s="2" t="s">
         <v>626</v>
       </c>
     </row>
@@ -7446,7 +7446,7 @@
       <c r="L129" t="s">
         <v>619</v>
       </c>
-      <c r="M129" s="3"/>
+      <c r="M129" s="2"/>
     </row>
     <row r="130" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
@@ -7485,7 +7485,7 @@
       <c r="L130" t="s">
         <v>619</v>
       </c>
-      <c r="M130" s="3" t="s">
+      <c r="M130" s="2" t="s">
         <v>626</v>
       </c>
     </row>
@@ -7526,7 +7526,7 @@
       <c r="L131" t="s">
         <v>619</v>
       </c>
-      <c r="M131" s="3"/>
+      <c r="M131" s="2"/>
     </row>
     <row r="132" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
@@ -7641,7 +7641,7 @@
       <c r="L134" t="s">
         <v>619</v>
       </c>
-      <c r="M134" s="3" t="s">
+      <c r="M134" s="2" t="s">
         <v>626</v>
       </c>
     </row>
@@ -7682,7 +7682,7 @@
       <c r="L135" t="s">
         <v>619</v>
       </c>
-      <c r="M135" s="3"/>
+      <c r="M135" s="2"/>
     </row>
     <row r="136" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
@@ -8028,7 +8028,7 @@
       <c r="L144" t="s">
         <v>619</v>
       </c>
-      <c r="M144" s="3" t="s">
+      <c r="M144" s="2" t="s">
         <v>626</v>
       </c>
     </row>
@@ -8069,7 +8069,7 @@
       <c r="L145" t="s">
         <v>619</v>
       </c>
-      <c r="M145" s="3"/>
+      <c r="M145" s="2"/>
     </row>
     <row r="146" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
@@ -8146,7 +8146,7 @@
       <c r="L147" t="s">
         <v>619</v>
       </c>
-      <c r="M147" s="3" t="s">
+      <c r="M147" s="2" t="s">
         <v>626</v>
       </c>
     </row>
@@ -8187,8 +8187,8 @@
       <c r="L148" t="s">
         <v>619</v>
       </c>
-      <c r="M148" s="3"/>
-      <c r="N148" s="3" t="s">
+      <c r="M148" s="2"/>
+      <c r="N148" s="2" t="s">
         <v>626</v>
       </c>
     </row>
@@ -8229,7 +8229,7 @@
       <c r="L149" t="s">
         <v>619</v>
       </c>
-      <c r="N149" s="3"/>
+      <c r="N149" s="2"/>
     </row>
     <row r="150" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
@@ -8306,7 +8306,7 @@
       <c r="L151" t="s">
         <v>619</v>
       </c>
-      <c r="M151" s="3" t="s">
+      <c r="M151" s="2" t="s">
         <v>626</v>
       </c>
     </row>
@@ -8347,7 +8347,7 @@
       <c r="L152" t="s">
         <v>619</v>
       </c>
-      <c r="M152" s="3"/>
+      <c r="M152" s="2"/>
     </row>
     <row r="153" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
@@ -8424,7 +8424,7 @@
       <c r="L154" t="s">
         <v>619</v>
       </c>
-      <c r="M154" s="3" t="s">
+      <c r="M154" s="2" t="s">
         <v>626</v>
       </c>
     </row>
@@ -8465,7 +8465,7 @@
       <c r="L155" t="s">
         <v>619</v>
       </c>
-      <c r="M155" s="3"/>
+      <c r="M155" s="2"/>
     </row>
     <row r="156" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
@@ -8542,7 +8542,7 @@
       <c r="L157" t="s">
         <v>619</v>
       </c>
-      <c r="M157" s="3" t="s">
+      <c r="M157" s="2" t="s">
         <v>626</v>
       </c>
     </row>
@@ -8583,7 +8583,7 @@
       <c r="L158" t="s">
         <v>619</v>
       </c>
-      <c r="M158" s="3"/>
+      <c r="M158" s="2"/>
     </row>
     <row r="159" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
@@ -8660,10 +8660,10 @@
       <c r="L160" t="s">
         <v>619</v>
       </c>
-      <c r="M160" s="3" t="s">
+      <c r="M160" s="2" t="s">
         <v>626</v>
       </c>
-      <c r="N160" s="3" t="s">
+      <c r="N160" s="2" t="s">
         <v>626</v>
       </c>
     </row>
@@ -8704,8 +8704,8 @@
       <c r="L161" t="s">
         <v>619</v>
       </c>
-      <c r="M161" s="3"/>
-      <c r="N161" s="3"/>
+      <c r="M161" s="2"/>
+      <c r="N161" s="2"/>
     </row>
     <row r="162" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
@@ -8744,7 +8744,7 @@
       <c r="L162" t="s">
         <v>619</v>
       </c>
-      <c r="M162" s="3" t="s">
+      <c r="M162" s="2" t="s">
         <v>626</v>
       </c>
     </row>
@@ -8785,7 +8785,7 @@
       <c r="L163" t="s">
         <v>619</v>
       </c>
-      <c r="M163" s="3"/>
+      <c r="M163" s="2"/>
     </row>
     <row r="164" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
@@ -8900,7 +8900,7 @@
       <c r="L166" t="s">
         <v>619</v>
       </c>
-      <c r="M166" s="3" t="s">
+      <c r="M166" s="2" t="s">
         <v>626</v>
       </c>
     </row>
@@ -8941,7 +8941,7 @@
       <c r="L167" t="s">
         <v>619</v>
       </c>
-      <c r="M167" s="3"/>
+      <c r="M167" s="2"/>
     </row>
     <row r="168" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
@@ -9474,7 +9474,7 @@
       <c r="L181" t="s">
         <v>619</v>
       </c>
-      <c r="M181" s="2" t="s">
+      <c r="M181" s="4" t="s">
         <v>671</v>
       </c>
     </row>
@@ -9515,7 +9515,7 @@
       <c r="L182" t="s">
         <v>619</v>
       </c>
-      <c r="M182" s="2"/>
+      <c r="M182" s="4"/>
     </row>
     <row r="183" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
@@ -9554,7 +9554,7 @@
       <c r="L183" t="s">
         <v>619</v>
       </c>
-      <c r="M183" s="2"/>
+      <c r="M183" s="4"/>
     </row>
     <row r="184" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
@@ -9745,7 +9745,7 @@
       <c r="L188" t="s">
         <v>619</v>
       </c>
-      <c r="M188" s="2" t="s">
+      <c r="M188" s="4" t="s">
         <v>671</v>
       </c>
     </row>
@@ -9786,7 +9786,7 @@
       <c r="L189" t="s">
         <v>620</v>
       </c>
-      <c r="M189" s="2"/>
+      <c r="M189" s="4"/>
     </row>
     <row r="190" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
@@ -9825,7 +9825,7 @@
       <c r="L190" t="s">
         <v>620</v>
       </c>
-      <c r="M190" s="2"/>
+      <c r="M190" s="4"/>
     </row>
     <row r="191" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
@@ -10058,6 +10058,43 @@
   </sheetData>
   <autoFilter ref="A1:K196" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <mergeCells count="45">
+    <mergeCell ref="M188:M190"/>
+    <mergeCell ref="M160:M161"/>
+    <mergeCell ref="N160:N161"/>
+    <mergeCell ref="M162:M163"/>
+    <mergeCell ref="M166:M167"/>
+    <mergeCell ref="M181:M183"/>
+    <mergeCell ref="M147:M148"/>
+    <mergeCell ref="N148:N149"/>
+    <mergeCell ref="M151:M152"/>
+    <mergeCell ref="M154:M155"/>
+    <mergeCell ref="M157:M158"/>
+    <mergeCell ref="M124:M125"/>
+    <mergeCell ref="M128:M129"/>
+    <mergeCell ref="M130:M131"/>
+    <mergeCell ref="M134:M135"/>
+    <mergeCell ref="M144:M145"/>
+    <mergeCell ref="M104:M105"/>
+    <mergeCell ref="M106:M107"/>
+    <mergeCell ref="M109:M110"/>
+    <mergeCell ref="M120:M121"/>
+    <mergeCell ref="M122:M123"/>
+    <mergeCell ref="M94:M95"/>
+    <mergeCell ref="M96:M97"/>
+    <mergeCell ref="M98:M100"/>
+    <mergeCell ref="M101:M102"/>
+    <mergeCell ref="N102:N103"/>
+    <mergeCell ref="M79:M81"/>
+    <mergeCell ref="M82:M86"/>
+    <mergeCell ref="M87:M88"/>
+    <mergeCell ref="M90:M91"/>
+    <mergeCell ref="M92:M93"/>
+    <mergeCell ref="M71:M72"/>
+    <mergeCell ref="M75:M76"/>
+    <mergeCell ref="M56:M57"/>
+    <mergeCell ref="M49:M50"/>
+    <mergeCell ref="M63:M64"/>
+    <mergeCell ref="M65:M66"/>
     <mergeCell ref="N65:N66"/>
     <mergeCell ref="O65:O66"/>
     <mergeCell ref="M8:M9"/>
@@ -10066,43 +10103,6 @@
     <mergeCell ref="M18:M19"/>
     <mergeCell ref="M20:M21"/>
     <mergeCell ref="N20:N21"/>
-    <mergeCell ref="M71:M72"/>
-    <mergeCell ref="M75:M76"/>
-    <mergeCell ref="M56:M57"/>
-    <mergeCell ref="M49:M50"/>
-    <mergeCell ref="M63:M64"/>
-    <mergeCell ref="M65:M66"/>
-    <mergeCell ref="M79:M81"/>
-    <mergeCell ref="M82:M86"/>
-    <mergeCell ref="M87:M88"/>
-    <mergeCell ref="M90:M91"/>
-    <mergeCell ref="M92:M93"/>
-    <mergeCell ref="M94:M95"/>
-    <mergeCell ref="M96:M97"/>
-    <mergeCell ref="M98:M100"/>
-    <mergeCell ref="M101:M102"/>
-    <mergeCell ref="N102:N103"/>
-    <mergeCell ref="M104:M105"/>
-    <mergeCell ref="M106:M107"/>
-    <mergeCell ref="M109:M110"/>
-    <mergeCell ref="M120:M121"/>
-    <mergeCell ref="M122:M123"/>
-    <mergeCell ref="M124:M125"/>
-    <mergeCell ref="M128:M129"/>
-    <mergeCell ref="M130:M131"/>
-    <mergeCell ref="M134:M135"/>
-    <mergeCell ref="M144:M145"/>
-    <mergeCell ref="M147:M148"/>
-    <mergeCell ref="N148:N149"/>
-    <mergeCell ref="M151:M152"/>
-    <mergeCell ref="M154:M155"/>
-    <mergeCell ref="M157:M158"/>
-    <mergeCell ref="M188:M190"/>
-    <mergeCell ref="M160:M161"/>
-    <mergeCell ref="N160:N161"/>
-    <mergeCell ref="M162:M163"/>
-    <mergeCell ref="M166:M167"/>
-    <mergeCell ref="M181:M183"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>